<commit_message>
renew test log 2013_12_22_18:40
</commit_message>
<xml_diff>
--- a/TestLog/动静一级OMP_CUDA_动态参数_实验测试表.xlsx
+++ b/TestLog/动静一级OMP_CUDA_动态参数_实验测试表.xlsx
@@ -408,7 +408,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -439,6 +439,12 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>13.946</v>
+      </c>
+      <c r="C3">
+        <v>41.671999999999997</v>
+      </c>
       <c r="D3">
         <v>252.02799999999999</v>
       </c>
@@ -448,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13.571999999999999</v>
+        <v>13.680999999999999</v>
       </c>
       <c r="C4">
         <v>24.399000000000001</v>
@@ -471,7 +477,10 @@
         <v>25.082999999999998</v>
       </c>
       <c r="D5">
-        <v>227.744</v>
+        <v>231.785</v>
+      </c>
+      <c r="E5">
+        <v>4492.3159999999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>